<commit_message>
Fall 2016 syllabus updates
</commit_message>
<xml_diff>
--- a/f16/setup/schedule.xlsx
+++ b/f16/setup/schedule.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26207"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bec/vc/pl/courses/csci3155/2015-fall/organization.IGNORE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bec/vc/bec/2016/3155-f16/csci3155.github.io/f16/setup/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="4200" windowWidth="28380" windowHeight="23780" tabRatio="500"/>
+    <workbookView xWindow="4280" yWindow="3360" windowWidth="32820" windowHeight="24300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule.csv" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -104,21 +104,12 @@
     <t>Collections and Callbacks (Higher-Order Functions)</t>
   </si>
   <si>
-    <t>Type Checking; Records. </t>
-  </si>
-  <si>
     <t>Procedural Abstraction. </t>
   </si>
   <si>
     <t>Variables and Pointers. Procedural Abstraction.</t>
   </si>
   <si>
-    <t>Continuations and Regular Expressions.</t>
-  </si>
-  <si>
-    <t>Parsing, Regular Expressions, and Continuations.</t>
-  </si>
-  <si>
     <t>Objects and Classes.</t>
   </si>
   <si>
@@ -128,25 +119,55 @@
     <t>No class. Thanksgiving break.</t>
   </si>
   <si>
-    <t>Lab 1 due 9/5</t>
-  </si>
-  <si>
-    <t>Lab  2 due 9/19</t>
-  </si>
-  <si>
-    <t>Lab 3 due 10/3</t>
-  </si>
-  <si>
-    <t>Lab 4 due 10/24</t>
-  </si>
-  <si>
-    <t>Lab 5 due 11/7</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
-    <t>Lab 6 due 11/21</t>
+    <t>Type Checking. Records. </t>
+  </si>
+  <si>
+    <t>Continuations. Regular Expressions.</t>
+  </si>
+  <si>
+    <t>Continuations. Regular Expressions. Parsing.</t>
+  </si>
+  <si>
+    <t>Project Presentations.</t>
+  </si>
+  <si>
+    <t>Lab 1 due</t>
+  </si>
+  <si>
+    <t>Lab 2 due</t>
+  </si>
+  <si>
+    <t>Lab 3 due</t>
+  </si>
+  <si>
+    <t>Lab 4 due</t>
+  </si>
+  <si>
+    <t>Lab 5 due</t>
+  </si>
+  <si>
+    <t>Lab 6 due</t>
+  </si>
+  <si>
+    <t>Exercise 1</t>
+  </si>
+  <si>
+    <t>Exercise 2</t>
+  </si>
+  <si>
+    <t>Exercise 3</t>
+  </si>
+  <si>
+    <t>Exercise 4</t>
+  </si>
+  <si>
+    <t>Exercise 6</t>
+  </si>
+  <si>
+    <t>Exercise 5</t>
   </si>
 </sst>
 </file>
@@ -764,7 +785,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -772,7 +793,7 @@
     <col min="1" max="2" width="2.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
@@ -798,7 +819,7 @@
         <v>T</v>
       </c>
       <c r="C2" s="2">
-        <v>40779</v>
+        <v>41143</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -806,26 +827,26 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="str">
-        <f>IF(C3="","",CHOOSE(WEEKDAY(C3),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" ref="B3:B6" si="0">IF(C3="","",CHOOSE(WEEKDAY(C3),"N","M","T","W","R","F","S"))</f>
+        <v>R</v>
       </c>
       <c r="C3" s="2">
-        <v>40780</v>
+        <v>41145</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="str">
-        <f t="shared" ref="B4:B7" si="0">IF(C4="","",CHOOSE(WEEKDAY(C4),"N","M","T","W","R","F","S"))</f>
-        <v>R</v>
+        <f>IF(C4="","",CHOOSE(WEEKDAY(C4),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C4" s="2">
-        <v>40781</v>
+        <v>41146</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -839,7 +860,7 @@
       </c>
       <c r="C5" s="2">
         <f>C2+7</f>
-        <v>40786</v>
+        <v>41150</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -851,15 +872,15 @@
         <v/>
       </c>
       <c r="B6" s="1" t="str">
-        <f>IF(C6="","",CHOOSE(WEEKDAY(C6),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="0"/>
+        <v>R</v>
       </c>
       <c r="C6" s="2">
         <f>C3+7</f>
-        <v>40787</v>
+        <v>41152</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -868,18 +889,18 @@
         <v/>
       </c>
       <c r="B7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>R</v>
+        <f>IF(C7="","",CHOOSE(WEEKDAY(C7),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C7" s="2">
         <f>C4+7</f>
-        <v>40788</v>
+        <v>41153</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -888,15 +909,18 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="str">
-        <f t="shared" ref="B8:B31" si="1">IF(C8="","",CHOOSE(WEEKDAY(C8),"N","M","T","W","R","F","S"))</f>
+        <f t="shared" ref="B8:B30" si="1">IF(C8="","",CHOOSE(WEEKDAY(C8),"N","M","T","W","R","F","S"))</f>
         <v>T</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" ref="C8:C49" si="2">C5+7</f>
-        <v>40793</v>
+        <f>C5+7</f>
+        <v>41157</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -905,15 +929,15 @@
         <v/>
       </c>
       <c r="B9" s="1" t="str">
-        <f>IF(C9="","",CHOOSE(WEEKDAY(C9),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="1"/>
+        <v>R</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="2"/>
-        <v>40794</v>
+        <f>C6+7</f>
+        <v>41159</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -922,15 +946,15 @@
         <v/>
       </c>
       <c r="B10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>R</v>
+        <f>IF(C10="","",CHOOSE(WEEKDAY(C10),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="2"/>
-        <v>40795</v>
+        <f>C7+7</f>
+        <v>41160</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -943,8 +967,8 @@
         <v>T</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="2"/>
-        <v>40800</v>
+        <f>C8+7</f>
+        <v>41164</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -956,15 +980,15 @@
         <v/>
       </c>
       <c r="B12" s="1" t="str">
-        <f>IF(C12="","",CHOOSE(WEEKDAY(C12),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="1"/>
+        <v>R</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="2"/>
-        <v>40801</v>
+        <f>C9+7</f>
+        <v>41166</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -973,18 +997,18 @@
         <v/>
       </c>
       <c r="B13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>R</v>
+        <f>IF(C13="","",CHOOSE(WEEKDAY(C13),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="2"/>
-        <v>40802</v>
+        <f>C10+7</f>
+        <v>41167</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -997,11 +1021,14 @@
         <v>T</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="2"/>
-        <v>40807</v>
+        <f>C11+7</f>
+        <v>41171</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -1010,15 +1037,15 @@
         <v/>
       </c>
       <c r="B15" s="1" t="str">
-        <f>IF(C15="","",CHOOSE(WEEKDAY(C15),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="1"/>
+        <v>R</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="2"/>
-        <v>40808</v>
+        <f>C12+7</f>
+        <v>41173</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -1027,15 +1054,15 @@
         <v/>
       </c>
       <c r="B16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>R</v>
+        <f>IF(C16="","",CHOOSE(WEEKDAY(C16),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="2"/>
-        <v>40809</v>
+        <f>C13+7</f>
+        <v>41174</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -1048,8 +1075,8 @@
         <v>T</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="2"/>
-        <v>40814</v>
+        <f>C14+7</f>
+        <v>41178</v>
       </c>
       <c r="D17" t="s">
         <v>24</v>
@@ -1061,15 +1088,15 @@
         <v/>
       </c>
       <c r="B18" s="1" t="str">
-        <f>IF(C18="","",CHOOSE(WEEKDAY(C18),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="1"/>
+        <v>R</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="2"/>
-        <v>40815</v>
+        <f>C15+7</f>
+        <v>41180</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -1078,18 +1105,18 @@
         <v/>
       </c>
       <c r="B19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>R</v>
+        <f>IF(C19="","",CHOOSE(WEEKDAY(C19),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="2"/>
-        <v>40816</v>
+        <f>C16+7</f>
+        <v>41181</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -1102,11 +1129,14 @@
         <v>T</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="2"/>
-        <v>40821</v>
+        <f>C17+7</f>
+        <v>41185</v>
       </c>
       <c r="D20" t="s">
         <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -1115,15 +1145,15 @@
         <v/>
       </c>
       <c r="B21" s="1" t="str">
-        <f>IF(C21="","",CHOOSE(WEEKDAY(C21),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="1"/>
+        <v>R</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="2"/>
-        <v>40822</v>
+        <f>C18+7</f>
+        <v>41187</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -1132,15 +1162,15 @@
         <v/>
       </c>
       <c r="B22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>R</v>
+        <f>IF(C22="","",CHOOSE(WEEKDAY(C22),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="2"/>
-        <v>40823</v>
+        <f>C19+7</f>
+        <v>41188</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
@@ -1153,8 +1183,8 @@
         <v>T</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="2"/>
-        <v>40828</v>
+        <f>C20+7</f>
+        <v>41192</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1166,15 +1196,15 @@
         <v/>
       </c>
       <c r="B24" s="1" t="str">
-        <f>IF(C24="","",CHOOSE(WEEKDAY(C24),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="1"/>
+        <v>R</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="2"/>
-        <v>40829</v>
+        <f>C21+7</f>
+        <v>41194</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -1183,15 +1213,15 @@
         <v/>
       </c>
       <c r="B25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>R</v>
+        <f>IF(C25="","",CHOOSE(WEEKDAY(C25),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="2"/>
-        <v>40830</v>
+        <f>C22+7</f>
+        <v>41195</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -1204,11 +1234,11 @@
         <v>T</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="2"/>
-        <v>40835</v>
+        <f>C23+7</f>
+        <v>41199</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
@@ -1217,15 +1247,15 @@
         <v/>
       </c>
       <c r="B27" s="1" t="str">
-        <f>IF(C27="","",CHOOSE(WEEKDAY(C27),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="1"/>
+        <v>R</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" si="2"/>
-        <v>40836</v>
+        <f>C24+7</f>
+        <v>41201</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
@@ -1234,18 +1264,18 @@
         <v/>
       </c>
       <c r="B28" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>R</v>
+        <f>IF(C28="","",CHOOSE(WEEKDAY(C28),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" si="2"/>
-        <v>40837</v>
+        <f>C25+7</f>
+        <v>41202</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
@@ -1258,11 +1288,14 @@
         <v>T</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="2"/>
-        <v>40842</v>
+        <f>C26+7</f>
+        <v>41206</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
+      </c>
+      <c r="F29" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -1271,15 +1304,15 @@
         <v/>
       </c>
       <c r="B30" s="1" t="str">
-        <f>IF(C30="","",CHOOSE(WEEKDAY(C30),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="1"/>
+        <v>R</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" si="2"/>
-        <v>40843</v>
+        <f>C27+7</f>
+        <v>41208</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -1288,15 +1321,15 @@
         <v/>
       </c>
       <c r="B31" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>R</v>
+        <f>IF(C31="","",CHOOSE(WEEKDAY(C31),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" si="2"/>
-        <v>40844</v>
+        <f>C28+7</f>
+        <v>41209</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -1304,15 +1337,15 @@
         <v>11</v>
       </c>
       <c r="B32" s="1" t="str">
-        <f t="shared" ref="B32:B49" si="3">IF(C32="","",CHOOSE(WEEKDAY(C32),"N","M","T","W","R","F","S"))</f>
+        <f t="shared" ref="B32:B48" si="2">IF(C32="","",CHOOSE(WEEKDAY(C32),"N","M","T","W","R","F","S"))</f>
         <v>T</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" si="2"/>
-        <v>40849</v>
+        <f>C29+7</f>
+        <v>41213</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
@@ -1321,15 +1354,15 @@
         <v/>
       </c>
       <c r="B33" s="1" t="str">
-        <f>IF(C33="","",CHOOSE(WEEKDAY(C33),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="2"/>
+        <v>R</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" si="2"/>
-        <v>40850</v>
+        <f>C30+7</f>
+        <v>41215</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
@@ -1338,18 +1371,18 @@
         <v/>
       </c>
       <c r="B34" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>R</v>
+        <f>IF(C34="","",CHOOSE(WEEKDAY(C34),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C34" s="2">
-        <f t="shared" si="2"/>
-        <v>40851</v>
+        <f>C31+7</f>
+        <v>41216</v>
       </c>
       <c r="D34" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
@@ -1358,15 +1391,18 @@
         <v>12</v>
       </c>
       <c r="B35" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="C35" s="2">
-        <f t="shared" si="2"/>
-        <v>40856</v>
+        <f>C32+7</f>
+        <v>41220</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="F35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
@@ -1375,15 +1411,15 @@
         <v/>
       </c>
       <c r="B36" s="1" t="str">
-        <f>IF(C36="","",CHOOSE(WEEKDAY(C36),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="2"/>
+        <v>R</v>
       </c>
       <c r="C36" s="2">
-        <f t="shared" si="2"/>
-        <v>40857</v>
+        <f>C33+7</f>
+        <v>41222</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
@@ -1392,15 +1428,15 @@
         <v/>
       </c>
       <c r="B37" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>R</v>
+        <f>IF(C37="","",CHOOSE(WEEKDAY(C37),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C37" s="2">
-        <f t="shared" si="2"/>
-        <v>40858</v>
+        <f>C34+7</f>
+        <v>41223</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -1409,32 +1445,32 @@
         <v>13</v>
       </c>
       <c r="B38" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="C38" s="2">
-        <f t="shared" si="2"/>
-        <v>40863</v>
+        <f>C35+7</f>
+        <v>41227</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" t="str">
-        <f>IF(A36="","",A36+1)</f>
+        <f t="shared" ref="A39" si="3">IF(A36="","",A36+1)</f>
         <v/>
       </c>
       <c r="B39" s="1" t="str">
-        <f>IF(C39="","",CHOOSE(WEEKDAY(C39),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="2"/>
+        <v>R</v>
       </c>
       <c r="C39" s="2">
-        <f t="shared" si="2"/>
-        <v>40864</v>
+        <f>C36+7</f>
+        <v>41229</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -1443,18 +1479,18 @@
         <v/>
       </c>
       <c r="B40" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>R</v>
+        <f>IF(C40="","",CHOOSE(WEEKDAY(C40),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C40" s="2">
-        <f t="shared" si="2"/>
-        <v>40865</v>
+        <f>C37+7</f>
+        <v>41230</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -1466,37 +1502,37 @@
         <v>T</v>
       </c>
       <c r="C41" s="2">
-        <f t="shared" si="2"/>
-        <v>40870</v>
+        <f>C38+7</f>
+        <v>41234</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="str">
         <f>IF(C42="","",CHOOSE(WEEKDAY(C42),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <v>R</v>
       </c>
       <c r="C42" s="2">
-        <f t="shared" si="2"/>
-        <v>40871</v>
+        <f>C39+7</f>
+        <v>41236</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="str">
         <f>IF(C43="","",CHOOSE(WEEKDAY(C43),"N","M","T","W","R","F","S"))</f>
-        <v>R</v>
+        <v>F</v>
       </c>
       <c r="C43" s="2">
-        <f t="shared" si="2"/>
-        <v>40872</v>
+        <f>C40+7</f>
+        <v>41237</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
@@ -1505,15 +1541,18 @@
         <v>14</v>
       </c>
       <c r="B44" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="C44" s="2">
-        <f t="shared" si="2"/>
-        <v>40877</v>
+        <f>C41+7</f>
+        <v>41241</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="F44" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
@@ -1522,15 +1561,15 @@
         <v/>
       </c>
       <c r="B45" s="1" t="str">
-        <f>IF(C45="","",CHOOSE(WEEKDAY(C45),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="2"/>
+        <v>R</v>
       </c>
       <c r="C45" s="2">
-        <f t="shared" si="2"/>
-        <v>40878</v>
+        <f>C42+7</f>
+        <v>41243</v>
       </c>
       <c r="D45" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
@@ -1539,12 +1578,12 @@
         <v/>
       </c>
       <c r="B46" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>R</v>
+        <f>IF(C46="","",CHOOSE(WEEKDAY(C46),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C46" s="2">
-        <f t="shared" si="2"/>
-        <v>40879</v>
+        <f>C43+7</f>
+        <v>41244</v>
       </c>
       <c r="D46" t="s">
         <v>31</v>
@@ -1556,15 +1595,15 @@
         <v>15</v>
       </c>
       <c r="B47" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="C47" s="2">
-        <f t="shared" si="2"/>
-        <v>40884</v>
+        <f>C44+7</f>
+        <v>41248</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
@@ -1573,12 +1612,12 @@
         <v/>
       </c>
       <c r="B48" s="1" t="str">
-        <f>IF(C48="","",CHOOSE(WEEKDAY(C48),"N","M","T","W","R","F","S"))</f>
-        <v>W</v>
+        <f t="shared" si="2"/>
+        <v>R</v>
       </c>
       <c r="C48" s="2">
-        <f t="shared" si="2"/>
-        <v>40885</v>
+        <f>C45+7</f>
+        <v>41250</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -1590,12 +1629,12 @@
         <v/>
       </c>
       <c r="B49" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>R</v>
+        <f>IF(C49="","",CHOOSE(WEEKDAY(C49),"N","M","T","W","R","F","S"))</f>
+        <v>F</v>
       </c>
       <c r="C49" s="2">
-        <f t="shared" si="2"/>
-        <v>40886</v>
+        <f>C46+7</f>
+        <v>41251</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>

</xml_diff>